<commit_message>
Updated info in forms regarding minor changes to the project
</commit_message>
<xml_diff>
--- a/Gantt chart project plan.csv.xlsx
+++ b/Gantt chart project plan.csv.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Go Diet App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{20C42B33-7378-4EFC-BF33-59E35E9B754A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BF415979-D866-448B-8F84-67568DC18541}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8976"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt chart project plan PROGRE" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="57" uniqueCount="52">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="56" uniqueCount="51">
   <si>
     <t>Phase Name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Description of the use of tools to support the development process</t>
   </si>
   <si>
-    <t>Description of any research hypothesis</t>
-  </si>
-  <si>
     <t>Bibliography</t>
   </si>
   <si>
@@ -191,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,23 +671,11 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="18" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="21" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="20" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -698,7 +683,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="21" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="20" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,7 +924,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -947,13 +944,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$E$3:$E$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$E$3:$E$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="46"/>
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
@@ -1049,7 +1046,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1298,16 +1295,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$49</c15:sqref>
                   </c15:fullRef>
                   <c15:levelRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$49</c15:sqref>
                   </c15:levelRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$49</c:f>
               <c:strCache>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>Ethical Forms</c:v>
                 </c:pt>
@@ -1438,15 +1435,12 @@
                   <c:v>Description of the use of tools to support the development process</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Description of any research hypothesis</c:v>
+                  <c:v>Bibliography</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>Bibliography</c:v>
+                  <c:v>Lessons learnt log</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>Lessons learnt log</c:v>
-                </c:pt>
-                <c:pt idx="46">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1454,10 +1448,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt chart project plan PROGRE'!$E$3:$E$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$E$3:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1554,16 +1548,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$49</c15:sqref>
                   </c15:fullRef>
                   <c15:levelRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$49</c15:sqref>
                   </c15:levelRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$49</c:f>
               <c:strCache>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>Ethical Forms</c:v>
                 </c:pt>
@@ -1694,15 +1688,12 @@
                   <c:v>Description of the use of tools to support the development process</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Description of any research hypothesis</c:v>
+                  <c:v>Bibliography</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>Bibliography</c:v>
+                  <c:v>Lessons learnt log</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>Lessons learnt log</c:v>
-                </c:pt>
-                <c:pt idx="46">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1710,10 +1701,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt chart project plan PROGRE'!$F$3:$F$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$F$3:$F$49</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="3">
                   <c:v>43394</c:v>
                 </c:pt>
@@ -1810,16 +1801,16 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$D$49</c15:sqref>
                   </c15:fullRef>
                   <c15:levelRef>
-                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$50</c15:sqref>
+                    <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$49</c15:sqref>
                   </c15:levelRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$C$3:$C$49</c:f>
               <c:strCache>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>Ethical Forms</c:v>
                 </c:pt>
@@ -1950,15 +1941,12 @@
                   <c:v>Description of the use of tools to support the development process</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Description of any research hypothesis</c:v>
+                  <c:v>Bibliography</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>Bibliography</c:v>
+                  <c:v>Lessons learnt log</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>Lessons learnt log</c:v>
-                </c:pt>
-                <c:pt idx="46">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1966,10 +1954,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt chart project plan PROGRE'!$G$3:$G$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$G$3:$G$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2240,6 +2228,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.3927904103667116E-3"/>
+          <c:y val="3.6363636363636362E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2271,7 +2267,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.6248650041506983E-2"/>
+          <c:y val="0.14438130170437558"/>
+          <c:w val="0.88675418585279187"/>
+          <c:h val="0.78701086414831045"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -2300,159 +2306,24 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt chart project plan PROGRE'!$C$4:$C$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$B$3:$B$49</c:f>
               <c:strCache>
-                <c:ptCount val="47"/>
-                <c:pt idx="0">
-                  <c:v>Ethical Forms</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Project Plan</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Global Checklist and BCS Checklist</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BCS Checklist</c:v>
-                </c:pt>
+                <c:ptCount val="22"/>
                 <c:pt idx="4">
-                  <c:v>Graphical User Interface feature</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Requirements Specification</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Documentation design</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Create, log in or remove account FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Researching and preparing recipes</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Designing how recipes are going to be selected</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Creating JSON file containing recipes</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>User inputs FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>`</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Periodic progress report</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Deliver data for classification algorithm</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Research and code classification algorithm</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Documentation, Testing</c:v>
+                  <c:v>Second Submission</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>User's selection feature</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Documentation, Testing</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Deliver data for weight loss predictions</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Code algorithm</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Code graphs and output to the user</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Output recipes to User FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Possibility to print recipes to PDF</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Testing, Documentation</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Enabling user to adjust the last input if wrong</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Application warning once when desired weight was achieved</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Lifecycle</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Description how verification and validation were applied</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Description of the use of tools to support the development process</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Description of any research hypothesis</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Bibliography</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Lessons learnt log</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Final Report</c:v>
+                  <c:v>Final Phase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt chart project plan PROGRE'!$D$3:$D$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$D$3:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="3">
                   <c:v>43374</c:v>
                 </c:pt>
@@ -2950,159 +2821,24 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Gantt chart project plan PROGRE'!$C$4:$C$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$B$3:$B$49</c:f>
               <c:strCache>
-                <c:ptCount val="47"/>
-                <c:pt idx="0">
-                  <c:v>Ethical Forms</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Project Plan</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Global Checklist and BCS Checklist</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BCS Checklist</c:v>
-                </c:pt>
+                <c:ptCount val="22"/>
                 <c:pt idx="4">
-                  <c:v>Graphical User Interface feature</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Requirements Specification</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Documentation design</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Create, log in or remove account FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Researching and preparing recipes</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Designing how recipes are going to be selected</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Creating JSON file containing recipes</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>User inputs FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>`</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Periodic progress report</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Deliver data for classification algorithm</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Research and code classification algorithm</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Documentation, Testing</c:v>
+                  <c:v>Second Submission</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>User's selection feature</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Documentation, Testing</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Deliver data for weight loss predictions</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Code algorithm</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Code graphs and output to the user</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Output recipes to User FEATURE</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Possibility to print recipes to PDF</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Testing, Documentation</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Enabling user to adjust the last input if wrong</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Application warning once when desired weight was achieved</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Lifecycle</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Description how verification and validation were applied</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Description of the use of tools to support the development process</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Description of any research hypothesis</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Bibliography</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Lessons learnt log</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Final Report</c:v>
+                  <c:v>Final Phase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gantt chart project plan PROGRE'!$E$3:$E$50</c:f>
+              <c:f>'Gantt chart project plan PROGRE'!$E$3:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
@@ -3219,152 +2955,17 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$4:$C$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="47"/>
-                      <c:pt idx="0">
-                        <c:v>Ethical Forms</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Project Plan</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Global Checklist and BCS Checklist</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>BCS Checklist</c:v>
-                      </c:pt>
+                      <c:ptCount val="22"/>
                       <c:pt idx="4">
-                        <c:v>Graphical User Interface feature</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Requirements Specification</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Documentation design</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Create, log in or remove account FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>Researching and preparing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>Designing how recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>Creating JSON file containing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>User inputs FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>`</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>Periodic progress report</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>Deliver data for classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>Research and code classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>Documentation, Testing</c:v>
+                        <c:v>Second Submission</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>User's selection feature</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>Documentation, Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>Deliver data for weight loss predictions</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>Code algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>Code graphs and output to the user</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>Output recipes to User FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>Possibility to print recipes to PDF</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>Testing, Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>Enabling user to adjust the last input if wrong</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>Application warning once when desired weight was achieved</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>Lifecycle</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>Description how verification and validation were applied</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>Description of the use of tools to support the development process</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>Description of any research hypothesis</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>Bibliography</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>Lessons learnt log</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>Final Report</c:v>
+                        <c:v>Final Phase</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3374,13 +2975,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="46"/>
                       <c:pt idx="4">
                         <c:v>0</c:v>
                       </c:pt>
@@ -3403,7 +3004,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Gantt chart project plan PROGRE'!$C$2</c15:sqref>
@@ -3433,168 +3034,33 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$4:$C$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="47"/>
-                      <c:pt idx="0">
-                        <c:v>Ethical Forms</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Project Plan</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Global Checklist and BCS Checklist</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>BCS Checklist</c:v>
-                      </c:pt>
+                      <c:ptCount val="22"/>
                       <c:pt idx="4">
-                        <c:v>Graphical User Interface feature</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Requirements Specification</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Documentation design</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Create, log in or remove account FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>Researching and preparing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>Designing how recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>Creating JSON file containing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>User inputs FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>`</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>Periodic progress report</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>Deliver data for classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>Research and code classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>Documentation, Testing</c:v>
+                        <c:v>Second Submission</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>User's selection feature</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>Documentation, Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>Deliver data for weight loss predictions</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>Code algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>Code graphs and output to the user</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>Output recipes to User FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>Possibility to print recipes to PDF</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>Testing, Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>Enabling user to adjust the last input if wrong</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>Application warning once when desired weight was achieved</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>Lifecycle</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>Description how verification and validation were applied</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>Description of the use of tools to support the development process</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>Description of any research hypothesis</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>Bibliography</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>Lessons learnt log</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>Final Report</c:v>
+                        <c:v>Final Phase</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$3:$C$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="46"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
@@ -3731,15 +3197,12 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="45">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
                         <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-CB65-404D-B0E5-7A87293F9958}"/>
                   </c:ext>
@@ -3752,7 +3215,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Gantt chart project plan PROGRE'!$F$2</c15:sqref>
@@ -3782,168 +3245,33 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$4:$C$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="47"/>
-                      <c:pt idx="0">
-                        <c:v>Ethical Forms</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Project Plan</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Global Checklist and BCS Checklist</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>BCS Checklist</c:v>
-                      </c:pt>
+                      <c:ptCount val="22"/>
                       <c:pt idx="4">
-                        <c:v>Graphical User Interface feature</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Requirements Specification</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Documentation design</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Create, log in or remove account FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>Researching and preparing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>Designing how recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>Creating JSON file containing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>User inputs FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>`</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>Periodic progress report</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>Deliver data for classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>Research and code classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>Documentation, Testing</c:v>
+                        <c:v>Second Submission</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>User's selection feature</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>Documentation, Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>Deliver data for weight loss predictions</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>Code algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>Code graphs and output to the user</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>Output recipes to User FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>Possibility to print recipes to PDF</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>Testing, Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>Enabling user to adjust the last input if wrong</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>Application warning once when desired weight was achieved</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>Lifecycle</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>Description how verification and validation were applied</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>Description of the use of tools to support the development process</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>Description of any research hypothesis</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>Bibliography</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>Lessons learnt log</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>Final Report</c:v>
+                        <c:v>Final Phase</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$F$3:$F$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$F$3:$F$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="46"/>
                       <c:pt idx="3">
                         <c:v>43394</c:v>
                       </c:pt>
@@ -4004,7 +3332,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-CB65-404D-B0E5-7A87293F9958}"/>
                   </c:ext>
@@ -4017,7 +3345,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Gantt chart project plan PROGRE'!$G$2</c15:sqref>
@@ -4047,168 +3375,33 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$C$4:$C$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$B$3:$B$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="47"/>
-                      <c:pt idx="0">
-                        <c:v>Ethical Forms</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Project Plan</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Global Checklist and BCS Checklist</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>BCS Checklist</c:v>
-                      </c:pt>
+                      <c:ptCount val="22"/>
                       <c:pt idx="4">
-                        <c:v>Graphical User Interface feature</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>Requirements Specification</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>Documentation design</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>Create, log in or remove account FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>Researching and preparing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>Designing how recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>Creating JSON file containing recipes</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>User inputs FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>`</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>Periodic progress report</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>Deliver data for classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>Research and code classification algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>Documentation, Testing</c:v>
+                        <c:v>Second Submission</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>If user is not qualified for weight loss, let him choose if he still wants to follow healthy lifestyle and keep using recipes for everyday</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>Define 3 paces of weight loss and predict how the recipes are going to be selected</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>User's selection feature</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>Documentation, Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>Deliver data for weight loss predictions</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>Predictive modelling Feature for outputting predicted weight loss in time</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>Code algorithm</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>Code graphs and output to the user</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>Output recipes to User FEATURE</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>Possibility to print recipes to PDF</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>Testing, Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>User day-to-day inputs recording and storing for outputting</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>Enabling user to adjust the last input if wrong</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>Outputting to the user his progress and further predictions based on his inputs as graph</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>Application warning once when desired weight was achieved</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>Choice for user if he wants to continue healthy diet adjusted to his new needs</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>Testing</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>Documentation</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>Lifecycle</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>Use Case Diagrams/Use Case Descriptions/Class diagrams</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>Description how verification and validation were applied</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>Description of the use of tools to support the development process</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>Description of any research hypothesis</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>Bibliography</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>Lessons learnt log</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>Final Report</c:v>
+                        <c:v>Final Phase</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Gantt chart project plan PROGRE'!$G$3:$G$50</c15:sqref>
+                          <c15:sqref>'Gantt chart project plan PROGRE'!$G$3:$G$49</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="47"/>
+                      <c:ptCount val="46"/>
                       <c:pt idx="3">
                         <c:v>3</c:v>
                       </c:pt>
@@ -4269,7 +3462,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-CB65-404D-B0E5-7A87293F9958}"/>
                   </c:ext>
@@ -4377,7 +3570,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4415,6 +3608,16 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0.15212733167712322"/>
+          <c:w val="9.4717477688656918E-2"/>
+          <c:h val="3.4177454400478424E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6119,13 +5322,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>519544</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6192,13 +5395,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>158748</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>103187</xdr:rowOff>
+      <xdr:rowOff>87312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>55562</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>198438</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6522,11 +5725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G50"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -6558,693 +5761,729 @@
       </c>
     </row>
     <row r="3" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="d">
+      <c r="D3" s="10" t="d">
         <f>DATE(2018, 10, 1)</f>
         <v>2018-10-01</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="d">
+      <c r="F3" s="10" t="d">
         <f>D3+E3</f>
         <v>2018-10-21</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="6" t="d">
+      <c r="B7" s="7"/>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3" t="d">
         <f>DATE(2018, 10, 1)</f>
         <v>2018-10-01</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="d">
+      <c r="F7" s="3" t="d">
         <f>D7+E7</f>
         <v>2018-10-21</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8" t="d">
+      <c r="D8" s="4" t="d">
         <f>DATE(2018, 10, 22)</f>
         <v>2018-10-22</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>14</v>
       </c>
-      <c r="F8" s="8" t="d">
+      <c r="F8" s="4" t="d">
         <f>D8+E8</f>
         <v>2018-11-05</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="d">
+      <c r="D11" s="4" t="d">
         <f>DATE(2018, 11, 4)</f>
         <v>2018-11-04</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>7</v>
       </c>
-      <c r="F11" s="8" t="d">
+      <c r="F11" s="4" t="d">
         <f>D11+E11</f>
         <v>2018-11-11</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="8" t="d">
+      <c r="D14" s="4" t="d">
         <f>DATE(2018, 11, 12)</f>
         <v>2018-11-12</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>7</v>
       </c>
-      <c r="F14" s="8" t="d">
+      <c r="F14" s="4" t="d">
         <f>D14+E14</f>
         <v>2018-11-19</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="6" t="d">
+      <c r="D16" s="3" t="d">
         <f>DATE(2018, 11, 12)</f>
         <v>2018-11-12</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>14</v>
       </c>
-      <c r="F16" s="6" t="d">
+      <c r="F16" s="3" t="d">
         <f>D16+E16</f>
         <v>2018-11-26</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="8" t="d">
+      <c r="D17" s="4" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="5">
         <v>14</v>
       </c>
-      <c r="F17" s="8" t="d">
+      <c r="F17" s="4" t="d">
         <f>D17+E17</f>
         <v>2018-12-10</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="8" t="d">
+      <c r="D20" s="4" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
         <v>7</v>
       </c>
-      <c r="F20" s="8" t="d">
+      <c r="F20" s="4" t="d">
         <f>D20+E20</f>
         <v>2018-12-03</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="8" t="d">
+      <c r="D22" s="4" t="d">
         <f>DATE(2018, 12, 10)</f>
         <v>2018-12-10</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>14</v>
       </c>
-      <c r="F22" s="8" t="d">
+      <c r="F22" s="4" t="d">
         <f>D22+E22</f>
         <v>2018-12-24</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="6" t="d">
+      <c r="D24" s="3" t="d">
         <f>DATE(2018, 12, 10)</f>
         <v>2018-12-10</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>7</v>
       </c>
-      <c r="F24" s="6" t="d">
+      <c r="F24" s="3" t="d">
         <f>D24+E24</f>
         <v>2018-12-17</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="6" t="d">
+      <c r="D25" s="3" t="d">
         <f>DATE(2019, 1, 7)</f>
         <v>2019-01-07</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>7</v>
       </c>
-      <c r="F25" s="6" t="d">
+      <c r="F25" s="3" t="d">
         <f>D25+E25</f>
         <v>2019-01-14</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="6" t="d">
+      <c r="D26" s="3" t="d">
         <f>DATE(2019, 1, 7)</f>
         <v>2019-01-07</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>14</v>
       </c>
-      <c r="F26" s="6" t="d">
+      <c r="F26" s="3" t="d">
         <f>D26+E26</f>
         <v>2019-01-21</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="8" t="d">
+      <c r="D27" s="4" t="d">
         <f>DATE(2019, 1, 7)</f>
         <v>2019-01-07</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="5">
         <v>7</v>
       </c>
-      <c r="F27" s="8" t="d">
+      <c r="F27" s="4" t="d">
         <f>D27+E27</f>
         <v>2019-01-14</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="8" t="d">
+      <c r="D29" s="4" t="d">
         <f>DATE(2019, 1, 21)</f>
         <v>2019-01-21</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="5">
         <v>14</v>
       </c>
-      <c r="F29" s="8" t="d">
+      <c r="F29" s="4" t="d">
         <f>D29+E29</f>
         <v>2019-02-04</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="9"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="8" t="d">
+      <c r="D33" s="4" t="d">
         <f>DATE(2019, 2, 4)</f>
         <v>2019-02-04</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="5">
         <v>7</v>
       </c>
-      <c r="F33" s="8" t="d">
+      <c r="F33" s="4" t="d">
         <f>D33+E33</f>
         <v>2019-02-11</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="10"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="10"/>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="10"/>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="8" t="d">
+      <c r="D36" s="4" t="d">
         <f>DATE(2019, 2, 11)</f>
         <v>2019-02-11</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="5">
         <v>7</v>
       </c>
-      <c r="F36" s="8" t="d">
+      <c r="F36" s="4" t="d">
         <f>D36+E36</f>
         <v>2019-02-18</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="10"/>
-      <c r="C37" s="3" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="9"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B38" s="10"/>
-      <c r="C38" s="3" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="10"/>
-      <c r="C39" s="3" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="8" t="d">
+      <c r="D39" s="4" t="d">
         <f>DATE(2019, 2, 18)</f>
         <v>2019-02-18</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="5">
         <v>7</v>
       </c>
-      <c r="F39" s="8" t="d">
+      <c r="F39" s="4" t="d">
         <f>D39+E39</f>
         <v>2019-02-25</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="10"/>
-      <c r="C40" s="3" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="9"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="9"/>
+      <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="8" t="d">
+      <c r="D41" s="4" t="d">
         <f>DATE(2019, 2, 22)</f>
         <v>2019-02-22</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="5">
         <v>30</v>
       </c>
-      <c r="F41" s="8" t="d">
+      <c r="F41" s="4" t="d">
         <f>D41+E41</f>
         <v>2019-03-24</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="10"/>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="10"/>
-      <c r="C43" s="3" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="6" t="d">
+      <c r="D43" s="3" t="d">
         <f>DATE(2019, 2, 25)</f>
         <v>2019-02-25</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>30</v>
       </c>
-      <c r="F43" s="6" t="d">
+      <c r="F43" s="3" t="d">
         <f>D43+E43</f>
         <v>2019-03-27</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="10"/>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="8" t="d">
+      <c r="D44" s="4" t="d">
         <f>DATE(2019, 2, 28)</f>
         <v>2019-02-28</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="5">
         <v>30</v>
       </c>
-      <c r="F44" s="8" t="d">
+      <c r="F44" s="4" t="d">
         <f>DATE(2019, 4, 5)</f>
         <v>2019-04-05</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="10"/>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B46" s="10"/>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="10"/>
-      <c r="C47" s="3" t="s">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="9"/>
+      <c r="C47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="10"/>
-      <c r="C48" s="3" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="9"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="10"/>
-      <c r="C49" s="3" t="s">
+      <c r="B49" s="9"/>
+      <c r="C49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="10"/>
-      <c r="C50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="9"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B8:B24"/>
+    <mergeCell ref="B25:B49"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="E44:E49"/>
+    <mergeCell ref="F44:F49"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G29:G32"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="E27:E28"/>
@@ -7256,54 +6495,8 @@
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:G23"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="E44:E50"/>
-    <mergeCell ref="F44:F50"/>
-    <mergeCell ref="G44:G50"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B8:B24"/>
-    <mergeCell ref="B25:B50"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D22:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>